<commit_message>
update web and CRUD
</commit_message>
<xml_diff>
--- a/Database/data.xlsx
+++ b/Database/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\FPT\PRJ301\PRJ301-BookShop\Database\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\FPT\PRJ301\PRJ301-BookShop\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3758F9AD-14DE-409E-8FF4-0DA3B53FEC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31248539-BE06-43CF-AC31-6368EEFF6486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,18 +50,12 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>Genre_id</t>
-  </si>
-  <si>
     <t>Publisher_id</t>
   </si>
   <si>
     <t>Author_id</t>
   </si>
   <si>
-    <t>Genres</t>
-  </si>
-  <si>
     <t>Publishers</t>
   </si>
   <si>
@@ -222,6 +216,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Category_id</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:I17"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,11 +655,11 @@
     <col min="4" max="4" width="21.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="1.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.21875" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="2.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="10.21875" style="1" bestFit="1" customWidth="1"/>
@@ -681,41 +681,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="O1" s="12"/>
       <c r="Q1" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="R1" s="8"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4">
         <v>108000</v>
@@ -724,13 +724,13 @@
         <v>100</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="4">
         <f>_xlfn.XLOOKUP(D2,L:L,K:K)</f>
@@ -748,24 +748,24 @@
         <v>1</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N2" s="10">
         <v>1</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="10">
         <v>1</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4">
         <v>79000</v>
@@ -774,13 +774,13 @@
         <v>100</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G3" s="4">
         <f t="shared" ref="G3:G17" si="0">_xlfn.XLOOKUP(D3,L:L,K:K)</f>
@@ -798,24 +798,24 @@
         <v>2</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N3" s="10">
         <v>2</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="10">
         <v>2</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4">
         <v>239000</v>
@@ -824,13 +824,13 @@
         <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" s="4">
         <f t="shared" si="0"/>
@@ -848,24 +848,24 @@
         <v>3</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N4" s="10">
         <v>3</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="10">
         <v>3</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4">
         <v>130000</v>
@@ -874,13 +874,13 @@
         <v>100</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" s="4">
         <f t="shared" si="0"/>
@@ -898,24 +898,24 @@
         <v>4</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N5" s="10">
         <v>4</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="10">
         <v>4</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4">
         <v>200000</v>
@@ -924,13 +924,13 @@
         <v>100</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
@@ -948,24 +948,24 @@
         <v>5</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N6" s="10">
         <v>5</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q6" s="10">
         <v>5</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4">
         <v>158000</v>
@@ -974,13 +974,13 @@
         <v>100</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
@@ -998,24 +998,24 @@
         <v>6</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N7" s="10">
         <v>6</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q7" s="10">
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4">
         <v>115000</v>
@@ -1024,13 +1024,13 @@
         <v>100</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
@@ -1048,24 +1048,24 @@
         <v>7</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="N8" s="10">
         <v>7</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Q8" s="10">
         <v>7</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4">
         <v>129000</v>
@@ -1074,13 +1074,13 @@
         <v>100</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
@@ -1098,24 +1098,24 @@
         <v>8</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N9" s="10">
         <v>8</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q9" s="10">
         <v>8</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
         <v>25000</v>
@@ -1124,13 +1124,13 @@
         <v>100</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
@@ -1148,18 +1148,18 @@
         <v>9</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q10" s="10">
         <v>9</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4">
         <v>25000</v>
@@ -1168,13 +1168,13 @@
         <v>100</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
@@ -1192,12 +1192,12 @@
         <v>10</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4">
         <v>499000</v>
@@ -1206,13 +1206,13 @@
         <v>100</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="0"/>
@@ -1230,12 +1230,12 @@
         <v>11</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4">
         <v>109000</v>
@@ -1244,13 +1244,13 @@
         <v>100</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
@@ -1268,12 +1268,12 @@
         <v>12</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="4">
         <v>31000</v>
@@ -1282,13 +1282,13 @@
         <v>100</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
@@ -1306,12 +1306,12 @@
         <v>13</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4">
         <v>145000</v>
@@ -1320,13 +1320,13 @@
         <v>100</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
@@ -1344,12 +1344,12 @@
         <v>14</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="4">
         <v>198000</v>
@@ -1358,13 +1358,13 @@
         <v>100</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B17" s="4">
         <v>158000</v>
@@ -1390,13 +1390,13 @@
         <v>100</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G17" s="4">
         <f t="shared" si="0"/>

</xml_diff>